<commit_message>
added more configuration to the amzon test
</commit_message>
<xml_diff>
--- a/documentation/Examples/WebNavigation/amazon.xlsx
+++ b/documentation/Examples/WebNavigation/amazon.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Amazon" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t xml:space="preserve">RUN</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve">Your Shopping Cart is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">import java.net.URL; import java.net.URLClassLoader; log.info("\nCLASSPATH:\n"); log.info(System.getProperty("java.class.path"));</t>
   </si>
 </sst>
 </file>
@@ -308,21 +311,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17:H17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.72448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.7602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -611,23 +613,34 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C18" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H18" s="0" t="s">
         <v>39</v>
       </c>
     </row>
@@ -636,7 +649,7 @@
     <hyperlink ref="C5" r:id="rId1" display="gpawel17@mail.com|1qazxsw2!"/>
     <hyperlink ref="H11" r:id="rId2" display="http://amazon.ca"/>
     <hyperlink ref="C13" r:id="rId3" display="gpawel17@mail.com|1qazxsw2!"/>
-    <hyperlink ref="H17" r:id="rId4" display="http://amazon.ca"/>
+    <hyperlink ref="H18" r:id="rId4" display="http://amazon.ca"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -653,15 +666,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="A17:H17 G1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="A17:C17 G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -681,13 +694,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -700,9 +716,12 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="1"/>
       <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
made a build. corrected mouse tests and pom version.
</commit_message>
<xml_diff>
--- a/documentation/Examples/WebNavigation/amazon.xlsx
+++ b/documentation/Examples/WebNavigation/amazon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="1" state="visible" r:id="rId2"/>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">enter user name and password</t>
   </si>
   <si>
-    <t xml:space="preserve">gpawel17@mail.com|1qazxsw2!</t>
+    <t xml:space="preserve">gpawel17@email.com|1Qazxsw2!</t>
   </si>
   <si>
     <t xml:space="preserve">xpath=//*[@id='nav-link-yourAccount']/span[1]</t>
@@ -189,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -232,6 +232,13 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -275,7 +282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -300,6 +307,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -319,19 +330,19 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,7 +426,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -569,14 +580,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -667,14 +678,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="gpawel17@mail.com|1qazxsw2!"/>
+    <hyperlink ref="C5" r:id="rId1" display="gpawel17@email.com"/>
     <hyperlink ref="H12" r:id="rId2" display="http://amazon.ca"/>
-    <hyperlink ref="C14" r:id="rId3" display="gpawel17@mail.com|1qazxsw2!"/>
+    <hyperlink ref="C14" r:id="rId3" display="gpawel17@email.com"/>
     <hyperlink ref="H19" r:id="rId4" display="http://amazon.ca"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -689,11 +700,14 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.62"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -744,7 +758,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
added loadProperties into FileUtils
</commit_message>
<xml_diff>
--- a/documentation/Examples/WebNavigation/amazon.xlsx
+++ b/documentation/Examples/WebNavigation/amazon.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t xml:space="preserve">RUN</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t xml:space="preserve">http://amazon.ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
   </si>
   <si>
     <t xml:space="preserve">Go to Cart</t>
@@ -189,7 +192,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -232,13 +235,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -282,7 +278,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -307,18 +303,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -331,7 +323,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -342,7 +334,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,9 +493,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>31</v>
@@ -518,7 +510,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>8</v>
       </c>
@@ -564,8 +556,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
+      <c r="A13" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -580,14 +572,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
+    <row r="14" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -599,30 +591,30 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>30</v>
@@ -630,24 +622,24 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>37</v>
@@ -658,7 +650,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>39</v>
@@ -678,9 +670,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="gpawel17@email.com"/>
+    <hyperlink ref="C5" r:id="rId1" display="gpawel17@email.com|1Qazxsw2!"/>
     <hyperlink ref="H12" r:id="rId2" display="http://amazon.ca"/>
-    <hyperlink ref="C14" r:id="rId3" display="gpawel17@email.com"/>
+    <hyperlink ref="C14" r:id="rId3" display="gpawel17@email.com|1Qazxsw2!"/>
     <hyperlink ref="H19" r:id="rId4" display="http://amazon.ca"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -749,7 +741,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>

</xml_diff>

<commit_message>
Added methods to DataProvider to provide TestNG style data.
</commit_message>
<xml_diff>
--- a/documentation/Examples/WebNavigation/amazon.xlsx
+++ b/documentation/Examples/WebNavigation/amazon.xlsx
@@ -287,10 +287,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -303,14 +299,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -320,10 +320,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -334,7 +334,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1018" min="7" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,8 +363,6 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -378,8 +377,6 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -390,12 +387,10 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -415,17 +410,15 @@
       </c>
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -437,8 +430,6 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -459,8 +450,6 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -503,7 +492,7 @@
       <c r="C9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="0" t="s">
@@ -517,7 +506,7 @@
       <c r="B10" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="0" t="s">
@@ -579,7 +568,7 @@
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -599,7 +588,7 @@
       <c r="C15" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -726,8 +715,8 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -744,8 +733,8 @@
         <v>53</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fixing some bugs and discovering more...
</commit_message>
<xml_diff>
--- a/documentation/Examples/WebNavigation/amazon.xlsx
+++ b/documentation/Examples/WebNavigation/amazon.xlsx
@@ -95,6 +95,9 @@
     <t xml:space="preserve">Showing results for</t>
   </si>
   <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
     <t xml:space="preserve">Extract first brush name</t>
   </si>
   <si>
@@ -147,9 +150,6 @@
   </si>
   <si>
     <t xml:space="preserve">http://amazon.ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
   </si>
   <si>
     <t xml:space="preserve">Go to Cart</t>
@@ -305,12 +305,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -322,8 +322,8 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -453,86 +453,86 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>14</v>
@@ -541,12 +541,12 @@
         <v>15</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>16</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>43</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>47</v>
@@ -606,12 +606,12 @@
         <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>49</v>
@@ -628,24 +628,24 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>14</v>
@@ -654,7 +654,7 @@
         <v>15</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
must fix load properies method
</commit_message>
<xml_diff>
--- a/documentation/Examples/WebNavigation/amazon.xlsx
+++ b/documentation/Examples/WebNavigation/amazon.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="72">
   <si>
     <t xml:space="preserve">RUN</t>
   </si>
@@ -182,7 +183,61 @@
     <t xml:space="preserve">Your Shopping Cart is empty</t>
   </si>
   <si>
-    <t xml:space="preserve">import java.net.URL; import java.net.URLClassLoader; log.info("\nCLASSPATH:\n"); log.info(System.getProperty("java.class.path"));</t>
+    <t xml:space="preserve">1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdfasdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asfaasdfas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdfasdfasdfa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdfa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fghmfg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asfdasdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fghjmfgjh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fghjfgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fghj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fghjfghj</t>
   </si>
 </sst>
 </file>
@@ -278,7 +333,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,10 +352,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -322,8 +373,8 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -679,18 +730,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,10 +766,209 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="986" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="987" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -729,12 +979,129 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
some fixes to ExpectedCondition and wait_pages_changes_stop.js script. Need to add on/off flags to the different wait condition methods.
</commit_message>
<xml_diff>
--- a/documentation/Examples/WebNavigation/amazon.xlsx
+++ b/documentation/Examples/WebNavigation/amazon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="1" state="visible" r:id="rId2"/>
@@ -356,12 +356,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -373,7 +373,7 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -732,7 +732,7 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated amazon.xlsx - all works at this moment.
</commit_message>
<xml_diff>
--- a/documentation/Examples/WebNavigation/amazon.xlsx
+++ b/documentation/Examples/WebNavigation/amazon.xlsx
@@ -96,42 +96,42 @@
     <t xml:space="preserve">Showing results for</t>
   </si>
   <si>
+    <t xml:space="preserve">Extract first brush name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xpath=//*[@id='atfResults']//li[1]//h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRUSH_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the first found item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;@!{xpath=//*[@id='atfResults']//li[1]//h2}&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${BRUSH_NAME}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on Add to Cart button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;@!{add-to-cart-button}&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xpath=//*[@id='huc-v2-order-row-confirm-text']/h1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added to Cart</t>
+  </si>
+  <si>
     <t xml:space="preserve">n</t>
   </si>
   <si>
-    <t xml:space="preserve">Extract first brush name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xpath=//*[@id='atfResults']//li[1]//h2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRUSH_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on the first found item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;@!{xpath=//*[@id='atfResults']//li[1]//h2}&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">productTitle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${BRUSH_NAME}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on Add to Cart button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;@!{add-to-cart-button}&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xpath=//*[@id='huc-v2-order-row-confirm-text']/h1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Added to Cart</t>
-  </si>
-  <si>
     <t xml:space="preserve">this is negative test</t>
   </si>
   <si>
@@ -147,7 +147,7 @@
     <t xml:space="preserve">Sign out</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;@!{nav-item-signout-sa}&gt;</t>
+    <t xml:space="preserve">&lt;@!{xpath=//span[contains(text(),'Sign Out')]}&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">http://amazon.ca</t>
@@ -374,7 +374,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -504,61 +504,61 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>37</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>38</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>40</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>16</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>43</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>47</v>
@@ -657,12 +657,12 @@
         <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>49</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>38</v>
@@ -688,9 +688,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>40</v>
@@ -868,7 +868,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>69</v>
@@ -882,7 +882,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>71</v>
@@ -891,7 +891,7 @@
         <v>70</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>69</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>71</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>69</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>71</v>
@@ -1080,7 +1080,7 @@
         <v>70</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>69</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>71</v>

</xml_diff>